<commit_message>
updated equipment list 2023
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2023.xlsx
+++ b/Kilroy Equipment List 2023.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="123">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>disableAutoSwitch</t>
-  </si>
-  <si>
-    <t>13 , 14, 15, 16, 17, 18</t>
   </si>
   <si>
     <r>
@@ -269,10 +266,142 @@
     <t>delaypot</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>delayPot</t>
+  </si>
+  <si>
+    <t>top left motor</t>
+  </si>
+  <si>
+    <t>top right motor</t>
+  </si>
+  <si>
+    <t>bottom left motor</t>
+  </si>
+  <si>
+    <t>bottom right motor</t>
+  </si>
+  <si>
+    <t>rightTopMotor</t>
+  </si>
+  <si>
+    <t>leftTopMotor</t>
+  </si>
+  <si>
+    <t>rightBottomMotor</t>
+  </si>
+  <si>
+    <t>leftBottomMotor</t>
+  </si>
+  <si>
+    <t>arm motor x</t>
+  </si>
+  <si>
+    <t>arm motor y</t>
+  </si>
+  <si>
+    <t>arm length</t>
+  </si>
+  <si>
+    <t>armMotorX</t>
+  </si>
+  <si>
+    <t>armMotorY</t>
+  </si>
+  <si>
+    <t>armMotorLength</t>
+  </si>
+  <si>
+    <t>ten turn potentiometer</t>
+  </si>
+  <si>
+    <t>tenPot</t>
+  </si>
+  <si>
+    <t>ebrake</t>
+  </si>
+  <si>
+    <t>eBrake</t>
+  </si>
+  <si>
+    <t>claw piston</t>
+  </si>
+  <si>
+    <t>clawPiston</t>
+  </si>
+  <si>
+    <t>e brake timer</t>
+  </si>
+  <si>
+    <t>eBrakeTimer</t>
+  </si>
+  <si>
+    <t>e brake timer stopped</t>
+  </si>
+  <si>
+    <t>eBrakeTimerIsStopped</t>
+  </si>
+  <si>
+    <t>automatic timer</t>
+  </si>
+  <si>
+    <t>autoTimer</t>
+  </si>
+  <si>
+    <t>left side motors</t>
+  </si>
+  <si>
+    <t>leftSideMotors</t>
+  </si>
+  <si>
+    <t>right side motors</t>
+  </si>
+  <si>
+    <t>rightSideMotors</t>
+  </si>
+  <si>
+    <t>transmission</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>cameras</t>
+  </si>
+  <si>
+    <t>camera switch</t>
+  </si>
+  <si>
+    <t>switchCamerViewButton10</t>
+  </si>
+  <si>
+    <t>switchCamerViewButton11</t>
+  </si>
+  <si>
+    <t>claw trigger</t>
+  </si>
+  <si>
+    <t>clawTriggerButton</t>
+  </si>
+  <si>
+    <t>14,15,16,17,19,20</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>6,7</t>
   </si>
 </sst>
 </file>
@@ -458,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -489,9 +618,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1005,8 +1131,8 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -1023,13 +1149,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.4">
       <c r="A2" s="5" t="s">
@@ -1051,10 +1177,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.2" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1062,1109 +1188,1219 @@
     <row r="4" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="61"/>
+      <c r="C4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="59"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="61"/>
-    </row>
-    <row r="7" spans="1:8" s="22" customFormat="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="59"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="21" customFormat="1">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="59"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="59"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="58"/>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="61"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="59"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="58"/>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="63"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="62"/>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="59"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="58"/>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="63"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="62"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="59"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="58"/>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="63"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="62"/>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="59"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="63"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="76" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="35" t="s">
+      <c r="D23" s="75"/>
+      <c r="E23" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="59"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="58"/>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="61"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="60"/>
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" s="4" customFormat="1">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="74" t="s">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="74"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="4" customFormat="1">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="28" t="s">
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="72" t="s">
+      <c r="D33" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="73">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="26.4">
+      <c r="E33" s="72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="61" t="s">
-        <v>73</v>
+      <c r="E34" s="60" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="4" customFormat="1">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="16"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="12"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="16"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="20"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5" s="4" customFormat="1">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="16"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" s="42" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="16"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="15"/>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5" s="42" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="16"/>
-    </row>
-    <row r="44" spans="1:5" s="42" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.2" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="20"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="74" t="s">
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="74"/>
+      <c r="D45" s="73"/>
       <c r="E45" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="4" customFormat="1">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="45"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
     </row>
     <row r="47" spans="1:5" s="4" customFormat="1">
-      <c r="A47" s="46"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="30"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="29"/>
     </row>
     <row r="48" spans="1:5" s="4" customFormat="1">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="16"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" s="4" customFormat="1">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="12"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A50" s="34"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="74" t="s">
+      <c r="A50" s="33"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="74"/>
+      <c r="D50" s="73"/>
       <c r="E50" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="42" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A51" s="48"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="64" t="s">
+    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.1" customHeight="1">
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E51" s="45" t="s">
-        <v>78</v>
+      <c r="E51" s="44" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="54"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="67"/>
+      <c r="A52" s="53"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="66" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="53" spans="1:5" s="4" customFormat="1">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="16"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:5" s="4" customFormat="1">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="12"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="11"/>
     </row>
     <row r="55" spans="1:5" s="4" customFormat="1">
-      <c r="A55" s="21"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="16"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" s="4" customFormat="1">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="12"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A57" s="34"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="74" t="s">
+      <c r="A57" s="33"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="74"/>
+      <c r="D57" s="73"/>
       <c r="E57" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="42" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A58" s="48"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="45"/>
+    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="44"/>
     </row>
     <row r="59" spans="1:5" s="4" customFormat="1">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="12"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" s="4" customFormat="1">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="16"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" s="4" customFormat="1">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="12"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="11"/>
     </row>
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A62" s="34"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="74" t="s">
+      <c r="A62" s="33"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="74"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="4" customFormat="1" ht="26.4">
-      <c r="A63" s="48"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="64" t="s">
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="D63" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="E63" s="59" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="64" spans="1:5" s="4" customFormat="1">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="12"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E64" s="60" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1">
-      <c r="A65" s="21"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="16"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="E65" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="66" spans="1:8" s="4" customFormat="1">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:8" s="50" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A67" s="21"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="16"/>
-      <c r="G67" s="51"/>
-      <c r="H67" s="51"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="15"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
     </row>
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="74" t="s">
+      <c r="A68" s="33"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="D68" s="74"/>
+      <c r="D68" s="73"/>
       <c r="E68" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="4" customFormat="1">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="38" t="s">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="39" t="s">
+      <c r="D69" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="4" customFormat="1">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="16"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="15"/>
     </row>
     <row r="71" spans="1:8" s="4" customFormat="1">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="12"/>
-    </row>
-    <row r="72" spans="1:8" s="50" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A72" s="21"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="16"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="11"/>
+    </row>
+    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A72" s="20"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="15"/>
+      <c r="G72" s="50"/>
+      <c r="H72" s="50"/>
     </row>
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="74" t="s">
+      <c r="A73" s="33"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D73" s="74"/>
+      <c r="D73" s="73"/>
       <c r="E73" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G73" s="52"/>
+      <c r="G73" s="51"/>
     </row>
     <row r="74" spans="1:8" s="4" customFormat="1">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="32" t="s">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="33" t="s">
+      <c r="D74" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G74" s="52"/>
+      <c r="G74" s="51"/>
     </row>
     <row r="75" spans="1:8" s="4" customFormat="1">
-      <c r="A75" s="21"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="28" t="s">
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G75" s="52"/>
+      <c r="G75" s="51"/>
     </row>
     <row r="76" spans="1:8" s="4" customFormat="1">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="30" t="s">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="31" t="s">
+      <c r="D76" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E76" s="20" t="s">
+      <c r="E76" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G76" s="52"/>
+      <c r="G76" s="51"/>
     </row>
     <row r="77" spans="1:8" s="4" customFormat="1">
-      <c r="A77" s="21"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="28" t="s">
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D77" s="29" t="s">
+      <c r="D77" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G77" s="52"/>
+      <c r="G77" s="51"/>
     </row>
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="74" t="s">
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="D78" s="74"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G78" s="52"/>
+      <c r="G78" s="51"/>
     </row>
     <row r="79" spans="1:8" s="4" customFormat="1">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="53"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="32"/>
-    </row>
-    <row r="80" spans="1:8" s="50" customFormat="1">
-      <c r="A80" s="21"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="60"/>
-      <c r="D80" s="62"/>
-      <c r="E80" s="59"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E79" s="31"/>
+    </row>
+    <row r="80" spans="1:8" s="49" customFormat="1">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="58"/>
     </row>
     <row r="81" spans="1:6" s="4" customFormat="1">
-      <c r="A81" s="54"/>
-      <c r="B81" s="54"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
+      <c r="A81" s="53"/>
+      <c r="B81" s="53"/>
+      <c r="C81" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D81" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="31"/>
     </row>
     <row r="82" spans="1:6" s="4" customFormat="1">
-      <c r="A82" s="21"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="59"/>
-      <c r="D82" s="62"/>
-      <c r="E82" s="59"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="58"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="58"/>
     </row>
     <row r="83" spans="1:6" s="4" customFormat="1">
-      <c r="A83" s="39"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="61"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E83" s="60" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="84" spans="1:6" s="4" customFormat="1">
-      <c r="A84" s="21"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="60"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="59"/>
-    </row>
-    <row r="85" spans="1:6" s="69" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A85" s="54"/>
-      <c r="B85" s="54"/>
-      <c r="C85" s="65"/>
-      <c r="D85" s="66"/>
-      <c r="E85" s="67"/>
-      <c r="F85" s="68"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="59"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="58"/>
+    </row>
+    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A85" s="53"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="64"/>
+      <c r="D85" s="65"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="67"/>
     </row>
     <row r="86" spans="1:6" s="4" customFormat="1">
-      <c r="A86" s="21"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="60"/>
-      <c r="D86" s="62"/>
-      <c r="E86" s="59"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="59"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="58"/>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.2" customHeight="1">
       <c r="A87" s="5"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="61"/>
-      <c r="F87" s="52"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="60"/>
+      <c r="F87" s="51"/>
     </row>
     <row r="88" spans="1:6" s="4" customFormat="1">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="60"/>
-      <c r="D88" s="62"/>
-      <c r="E88" s="59"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="59"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="58"/>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="53"/>
-      <c r="F89" s="52"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="31"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="52"/>
+      <c r="F89" s="51"/>
     </row>
     <row r="90" spans="1:6" s="4" customFormat="1">
-      <c r="A90" s="21"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="60"/>
-      <c r="D90" s="62"/>
-      <c r="E90" s="59"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="58"/>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.2" customHeight="1">
       <c r="A91" s="5"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="61"/>
-      <c r="F91" s="52"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="60"/>
+      <c r="F91" s="51"/>
     </row>
     <row r="92" spans="1:6" s="4" customFormat="1">
-      <c r="A92" s="21"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="60"/>
-      <c r="D92" s="62"/>
-      <c r="E92" s="59"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="59"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="58"/>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.2" customHeight="1">
       <c r="A93" s="5"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="52"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="31"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="60"/>
+      <c r="F93" s="51"/>
     </row>
     <row r="94" spans="1:6" s="4" customFormat="1">
-      <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="60"/>
-      <c r="D94" s="62"/>
-      <c r="E94" s="59"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="59"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="58"/>
     </row>
     <row r="95" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A95" s="5"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="61"/>
-      <c r="F95" s="52"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="31"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="60"/>
+      <c r="F95" s="51"/>
     </row>
     <row r="96" spans="1:6" s="4" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A96" s="21"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="29"/>
-      <c r="E96" s="16"/>
+      <c r="A96" s="20"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="15"/>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="13.2" customHeight="1">
       <c r="A97" s="5"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="31"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="52"/>
+      <c r="B97" s="16"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="51"/>
     </row>
     <row r="98" spans="1:7" s="4" customFormat="1">
-      <c r="A98" s="21"/>
-      <c r="B98" s="21"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="16"/>
+      <c r="A98" s="20"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="15"/>
     </row>
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A99" s="34"/>
-      <c r="B99" s="34"/>
-      <c r="C99" s="74" t="s">
+      <c r="A99" s="33"/>
+      <c r="B99" s="33"/>
+      <c r="C99" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D99" s="74"/>
+      <c r="D99" s="73"/>
       <c r="E99" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G99" s="52"/>
+      <c r="G99" s="51"/>
     </row>
     <row r="100" spans="1:7" s="4" customFormat="1">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="53" t="s">
+      <c r="A100" s="16"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="D100" s="39" t="s">
+      <c r="D100" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E100" s="38" t="s">
+      <c r="E100" s="37" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="4" customFormat="1">
-      <c r="A101" s="21"/>
-      <c r="B101" s="21"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="16"/>
+      <c r="A101" s="20"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="15"/>
     </row>
     <row r="102" spans="1:7" s="4" customFormat="1">
-      <c r="A102" s="34"/>
-      <c r="B102" s="34"/>
-      <c r="C102" s="35" t="s">
+      <c r="A102" s="33"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D102" s="55"/>
-      <c r="E102" s="35" t="s">
+      <c r="D102" s="54"/>
+      <c r="E102" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
-      <c r="C103" s="32" t="s">
+      <c r="C103" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D103" s="33" t="s">
+      <c r="D103" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E103" s="61" t="s">
+      <c r="E103" s="60" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="4" customFormat="1">
-      <c r="A104" s="21"/>
-      <c r="B104" s="21"/>
-      <c r="C104" s="60" t="s">
+      <c r="A104" s="20"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D104" s="29" t="s">
+      <c r="D104" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="E104" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
-      <c r="C105" s="38" t="s">
+      <c r="C105" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D105" s="33" t="s">
+      <c r="D105" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E105" s="56" t="s">
+      <c r="E105" s="55" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="4" customFormat="1">
-      <c r="A106" s="21"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="28" t="s">
+      <c r="A106" s="20"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D106" s="29" t="s">
+      <c r="D106" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E106" s="57" t="s">
+      <c r="E106" s="56" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="33"/>
-      <c r="E107" s="61"/>
+      <c r="C107" s="31"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="60"/>
     </row>
     <row r="108" spans="1:7" s="4" customFormat="1">
-      <c r="A108" s="21"/>
-      <c r="B108" s="21"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="29"/>
-      <c r="E108" s="16"/>
+      <c r="A108" s="20"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="15"/>
     </row>
     <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
-      <c r="C109" s="30" t="s">
+      <c r="C109" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D109" s="31" t="s">
+      <c r="D109" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E109" s="20" t="s">
+      <c r="E109" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="4" customFormat="1">
-      <c r="A110" s="21"/>
-      <c r="B110" s="21"/>
-      <c r="C110" s="28" t="s">
+      <c r="A110" s="20"/>
+      <c r="B110" s="20"/>
+      <c r="C110" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D110" s="29" t="s">
+      <c r="D110" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="E110" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
-      <c r="C111" s="30" t="s">
+      <c r="C111" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D111" s="33" t="s">
+      <c r="D111" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="E111" s="30" t="s">
+      <c r="E111" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="4" customFormat="1">
-      <c r="A112" s="21"/>
-      <c r="B112" s="21"/>
-      <c r="C112" s="28" t="s">
+      <c r="A112" s="20"/>
+      <c r="B112" s="20"/>
+      <c r="C112" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D112" s="29" t="s">
+      <c r="D112" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E112" s="16" t="s">
+      <c r="E112" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
-      <c r="C113" s="70"/>
-      <c r="D113" s="66"/>
-      <c r="E113" s="67"/>
+      <c r="C113" s="69"/>
+      <c r="D113" s="65"/>
+      <c r="E113" s="66"/>
     </row>
     <row r="114" spans="1:5" s="4" customFormat="1">
-      <c r="A114" s="21"/>
-      <c r="B114" s="21"/>
-      <c r="C114" s="60"/>
-      <c r="D114" s="62"/>
-      <c r="E114" s="59"/>
+      <c r="A114" s="20"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D114" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="E114" s="58" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="115" spans="1:5" s="4" customFormat="1">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="32"/>
-      <c r="D115" s="33"/>
-      <c r="E115" s="61"/>
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E115" s="60"/>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1">
-      <c r="A116" s="21"/>
-      <c r="B116" s="21"/>
-      <c r="C116" s="60"/>
-      <c r="D116" s="62"/>
-      <c r="E116" s="59"/>
+      <c r="A116" s="20"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D116" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="E116" s="58"/>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="32"/>
-      <c r="D117" s="33"/>
-      <c r="E117" s="61"/>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="31"/>
+      <c r="D117" s="32"/>
+      <c r="E117" s="60"/>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="21"/>
-      <c r="B118" s="21"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="29"/>
-      <c r="E118" s="16"/>
-    </row>
-    <row r="119" spans="1:5" s="4" customFormat="1">
-      <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="38"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="20"/>
-    </row>
-    <row r="120" spans="1:5" s="4" customFormat="1">
-      <c r="A120" s="21"/>
-      <c r="B120" s="21"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="29"/>
-      <c r="E120" s="16"/>
+      <c r="A118" s="20"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="D118" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E118" s="15"/>
+    </row>
+    <row r="119" spans="1:5" s="4" customFormat="1" ht="26.4">
+      <c r="A119" s="16"/>
+      <c r="B119" s="16"/>
+      <c r="C119" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D119" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E119" s="19"/>
+    </row>
+    <row r="120" spans="1:5" s="4" customFormat="1" ht="26.4">
+      <c r="A120" s="20"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="D120" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E120" s="15"/>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="38"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="20"/>
+      <c r="A121" s="16"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="38"/>
+      <c r="E121" s="19"/>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1">
-      <c r="A122" s="21"/>
-      <c r="B122" s="21"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="29"/>
-      <c r="E122" s="16"/>
+      <c r="A122" s="20"/>
+      <c r="B122" s="20"/>
+      <c r="C122" s="27"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="15"/>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="38"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="20"/>
+      <c r="A123" s="16"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="37"/>
+      <c r="D123" s="38"/>
+      <c r="E123" s="19"/>
     </row>
     <row r="124" spans="1:5" s="4" customFormat="1">
-      <c r="A124" s="21"/>
-      <c r="B124" s="21"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="29"/>
-      <c r="E124" s="16"/>
+      <c r="A124" s="20"/>
+      <c r="B124" s="20"/>
+      <c r="C124" s="27"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="15"/>
     </row>
     <row r="125" spans="1:5" s="4" customFormat="1">
-      <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="38"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="20"/>
+      <c r="A125" s="16"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="38"/>
+      <c r="E125" s="19"/>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1">
-      <c r="A126" s="21"/>
-      <c r="B126" s="21"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="29"/>
-      <c r="E126" s="16"/>
+      <c r="A126" s="20"/>
+      <c r="B126" s="20"/>
+      <c r="C126" s="27"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="15"/>
     </row>
     <row r="127" spans="1:5" s="4" customFormat="1">
-      <c r="A127" s="17"/>
-      <c r="B127" s="17"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="20"/>
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="37"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="19"/>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1">
-      <c r="A128" s="21"/>
-      <c r="B128" s="21"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="29"/>
-      <c r="E128" s="16"/>
+      <c r="A128" s="20"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="27"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="15"/>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
-      <c r="C129" s="30" t="s">
+      <c r="C129" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D129" s="31" t="s">
+      <c r="D129" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E129" s="30" t="s">
+      <c r="E129" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1">
-      <c r="A130" s="21"/>
-      <c r="B130" s="21"/>
-      <c r="C130" s="28" t="s">
+      <c r="A130" s="20"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D130" s="29" t="s">
+      <c r="D130" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E130" s="16" t="s">
+      <c r="E130" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2173,560 +2409,560 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="58"/>
+      <c r="E131" s="57"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="58"/>
+      <c r="E132" s="57"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="58"/>
+      <c r="E133" s="57"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="58"/>
+      <c r="E134" s="57"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="58"/>
+      <c r="E135" s="57"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="58"/>
+      <c r="E136" s="57"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="58"/>
+      <c r="E137" s="57"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="58"/>
+      <c r="E138" s="57"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="58"/>
+      <c r="E139" s="57"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="58"/>
+      <c r="E140" s="57"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="58"/>
+      <c r="E141" s="57"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="58"/>
+      <c r="E142" s="57"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="58"/>
+      <c r="E143" s="57"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="58"/>
+      <c r="E144" s="57"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="58"/>
+      <c r="E145" s="57"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="58"/>
+      <c r="E146" s="57"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="58"/>
+      <c r="E147" s="57"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="58"/>
+      <c r="E148" s="57"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="58"/>
+      <c r="E149" s="57"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="58"/>
+      <c r="E150" s="57"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="58"/>
+      <c r="E151" s="57"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="58"/>
+      <c r="E152" s="57"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="58"/>
+      <c r="E153" s="57"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="58"/>
+      <c r="E154" s="57"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="58"/>
+      <c r="E155" s="57"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="58"/>
+      <c r="E156" s="57"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="58"/>
+      <c r="E157" s="57"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="58"/>
+      <c r="E158" s="57"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="58"/>
+      <c r="E159" s="57"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="58"/>
+      <c r="E160" s="57"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="58"/>
+      <c r="E161" s="57"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="58"/>
+      <c r="E162" s="57"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="58"/>
+      <c r="E163" s="57"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="58"/>
+      <c r="E164" s="57"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="58"/>
+      <c r="E165" s="57"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="58"/>
+      <c r="E166" s="57"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="58"/>
+      <c r="E167" s="57"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="58"/>
+      <c r="E168" s="57"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="58"/>
+      <c r="E169" s="57"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="58"/>
+      <c r="E170" s="57"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="58"/>
+      <c r="E171" s="57"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="58"/>
+      <c r="E172" s="57"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="58"/>
+      <c r="E173" s="57"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="58"/>
+      <c r="E174" s="57"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="58"/>
+      <c r="E175" s="57"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="58"/>
+      <c r="E176" s="57"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="58"/>
+      <c r="E177" s="57"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="58"/>
+      <c r="E178" s="57"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="58"/>
+      <c r="E179" s="57"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="58"/>
+      <c r="E180" s="57"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="58"/>
+      <c r="E181" s="57"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="58"/>
+      <c r="E182" s="57"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="58"/>
+      <c r="E183" s="57"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="58"/>
+      <c r="E184" s="57"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="58"/>
+      <c r="E185" s="57"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="58"/>
+      <c r="E186" s="57"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="58"/>
+      <c r="E187" s="57"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="58"/>
+      <c r="E188" s="57"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="58"/>
+      <c r="E189" s="57"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="58"/>
+      <c r="E190" s="57"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="58"/>
+      <c r="E191" s="57"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="58"/>
+      <c r="E192" s="57"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="58"/>
+      <c r="E193" s="57"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="58"/>
+      <c r="E194" s="57"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="58"/>
+      <c r="E195" s="57"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="58"/>
+      <c r="E196" s="57"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
-      <c r="E197" s="58"/>
+      <c r="E197" s="57"/>
     </row>
     <row r="198" spans="1:5" s="4" customFormat="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
-      <c r="E198" s="58"/>
+      <c r="E198" s="57"/>
     </row>
     <row r="199" spans="1:5" s="4" customFormat="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
-      <c r="E199" s="58"/>
+      <c r="E199" s="57"/>
     </row>
     <row r="200" spans="1:5" s="4" customFormat="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
-      <c r="E200" s="58"/>
+      <c r="E200" s="57"/>
     </row>
     <row r="201" spans="1:5" s="4" customFormat="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
-      <c r="E201" s="58"/>
+      <c r="E201" s="57"/>
     </row>
     <row r="202" spans="1:5" s="4" customFormat="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
-      <c r="E202" s="58"/>
+      <c r="E202" s="57"/>
     </row>
     <row r="203" spans="1:5" s="4" customFormat="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
-      <c r="E203" s="58"/>
+      <c r="E203" s="57"/>
     </row>
     <row r="204" spans="1:5" s="4" customFormat="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
-      <c r="E204" s="58"/>
+      <c r="E204" s="57"/>
     </row>
     <row r="205" spans="1:5" s="4" customFormat="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
-      <c r="E205" s="58"/>
+      <c r="E205" s="57"/>
     </row>
     <row r="206" spans="1:5" s="4" customFormat="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
-      <c r="E206" s="58"/>
+      <c r="E206" s="57"/>
     </row>
     <row r="207" spans="1:5" s="4" customFormat="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
-      <c r="E207" s="58"/>
+      <c r="E207" s="57"/>
     </row>
     <row r="208" spans="1:5" s="4" customFormat="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
-      <c r="E208" s="58"/>
+      <c r="E208" s="57"/>
     </row>
     <row r="209" spans="1:5" s="4" customFormat="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
-      <c r="E209" s="58"/>
+      <c r="E209" s="57"/>
     </row>
     <row r="210" spans="1:5" s="4" customFormat="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
-      <c r="E210" s="58"/>
+      <c r="E210" s="57"/>
     </row>
     <row r="211" spans="1:5" s="4" customFormat="1">
       <c r="A211" s="1"/>

</xml_diff>

<commit_message>
updates to the equipment list
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2023.xlsx
+++ b/Kilroy Equipment List 2023.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="150">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -461,9 +461,6 @@
     <t>n/a Ln210</t>
   </si>
   <si>
-    <t xml:space="preserve">arm motor </t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -473,7 +470,19 @@
     <t>Six Position Switch (2023)</t>
   </si>
   <si>
-    <t>13,,14,15,16,17,18</t>
+    <t>13,14,15,16,17,18</t>
+  </si>
+  <si>
+    <t>armRaiseMotor</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>armRaiseMotor - CAN Venom</t>
+  </si>
+  <si>
+    <t>armLengthMotor - Victor_SPX</t>
   </si>
 </sst>
 </file>
@@ -877,11 +886,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1192,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1203,8 +1212,8 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
@@ -1221,13 +1230,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
@@ -1249,10 +1258,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.25" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1404,21 +1413,27 @@
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="59" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D15" s="61" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="62"/>
+      <c r="C16" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="20"/>
@@ -1550,10 +1565,10 @@
     <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="73"/>
+      <c r="D32" s="74"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
@@ -1575,7 +1590,7 @@
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>70</v>
@@ -1588,13 +1603,13 @@
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D35" s="39" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
@@ -1663,10 +1678,10 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="73"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="9" t="s">
         <v>13</v>
       </c>
@@ -1710,10 +1725,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="9" t="s">
         <v>16</v>
       </c>
@@ -1775,10 +1790,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
       <c r="A57" s="33"/>
       <c r="B57" s="33"/>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="9" t="s">
         <v>18</v>
       </c>
@@ -1814,10 +1829,10 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="33"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="9" t="s">
         <v>20</v>
       </c>
@@ -1880,10 +1895,10 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="33"/>
       <c r="B68" s="33"/>
-      <c r="C68" s="73" t="s">
+      <c r="C68" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="73"/>
+      <c r="D68" s="74"/>
       <c r="E68" s="9" t="s">
         <v>22</v>
       </c>
@@ -1927,10 +1942,10 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="33"/>
       <c r="B73" s="33"/>
-      <c r="C73" s="73" t="s">
+      <c r="C73" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="73"/>
+      <c r="D73" s="74"/>
       <c r="E73" s="9" t="s">
         <v>26</v>
       </c>
@@ -1995,10 +2010,10 @@
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="33"/>
       <c r="B78" s="33"/>
-      <c r="C78" s="73" t="s">
+      <c r="C78" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="73"/>
+      <c r="D78" s="74"/>
       <c r="E78" s="9" t="s">
         <v>39</v>
       </c>
@@ -2202,10 +2217,10 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="33"/>
       <c r="B99" s="33"/>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D99" s="73"/>
+      <c r="D99" s="74"/>
       <c r="E99" s="9" t="s">
         <v>39</v>
       </c>
@@ -3411,11 +3426,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3423,6 +3433,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added some working code for autonomous
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2023.xlsx
+++ b/Kilroy Equipment List 2023.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="150">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>0,1</t>
+  </si>
+  <si>
+    <t>redLightSensor</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Red light sensor - QS18VN6LV</t>
   </si>
 </sst>
 </file>
@@ -860,11 +869,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1175,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1186,33 +1195,32 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14:E14"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.6328125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="1"/>
-    <col min="8" max="8" width="11.08984375" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.90625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1229,13 +1237,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="21" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="21" customFormat="1">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="13" t="s">
@@ -1292,7 +1300,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
@@ -1302,7 +1310,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="59" t="s">
@@ -1318,7 +1326,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="31" t="s">
@@ -1334,7 +1342,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="59" t="s">
@@ -1347,7 +1355,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="31" t="s">
@@ -1363,21 +1371,21 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="59"/>
       <c r="D13" s="61"/>
       <c r="E13" s="58"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="60"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="59" t="s">
@@ -1390,7 +1398,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="31" t="s">
@@ -1403,49 +1411,49 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="59"/>
       <c r="D17" s="61"/>
       <c r="E17" s="58"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="62"/>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="19" spans="1:8" s="4" customFormat="1">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="59"/>
       <c r="D19" s="61"/>
       <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="46"/>
       <c r="D20" s="70"/>
       <c r="E20" s="62"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="59"/>
       <c r="D21" s="61"/>
       <c r="E21" s="58"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="46"/>
       <c r="D22" s="70"/>
       <c r="E22" s="62"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="33"/>
       <c r="C23" s="75" t="s">
@@ -1456,21 +1464,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="58"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="C24" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="31"/>
       <c r="D25" s="32"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="59"/>
@@ -1480,7 +1494,7 @@
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="31"/>
@@ -1490,7 +1504,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="28" spans="1:8" s="4" customFormat="1">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="59"/>
@@ -1500,7 +1514,7 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="31"/>
@@ -1510,7 +1524,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="27"/>
@@ -1520,7 +1534,7 @@
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="37"/>
@@ -1530,18 +1544,18 @@
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="73"/>
+      <c r="D32" s="74"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="36"/>
       <c r="B33" s="36"/>
       <c r="C33" s="27" t="s">
@@ -1554,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="31" t="s">
@@ -1567,7 +1581,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="59" t="s">
@@ -1580,81 +1594,81 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="29"/>
       <c r="D36" s="30"/>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="31"/>
       <c r="D38" s="40"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="29"/>
       <c r="D40" s="30"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="37"/>
       <c r="D42" s="38"/>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="27"/>
       <c r="D43" s="28"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="29"/>
       <c r="D44" s="30"/>
       <c r="E44" s="19"/>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="73"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="42" t="s">
         <v>14</v>
       </c>
@@ -1672,7 +1686,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="29"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="20" t="s">
         <v>14</v>
       </c>
@@ -1683,25 +1697,25 @@
       <c r="D48" s="28"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="37"/>
       <c r="D49" s="38"/>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.15" customHeight="1">
+    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.1" customHeight="1">
       <c r="A51" s="47"/>
       <c r="B51" s="47"/>
       <c r="C51" s="63" t="s">
@@ -1714,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="53"/>
       <c r="B52" s="53"/>
       <c r="C52" s="69" t="s">
@@ -1727,92 +1741,92 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="27"/>
       <c r="D53" s="28"/>
       <c r="E53" s="15"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="16"/>
       <c r="B54" s="16"/>
       <c r="C54" s="31"/>
       <c r="D54" s="32"/>
       <c r="E54" s="11"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="27"/>
       <c r="D55" s="28"/>
       <c r="E55" s="15"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="31"/>
       <c r="D56" s="32"/>
       <c r="E56" s="11"/>
     </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A57" s="33"/>
       <c r="B57" s="33"/>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A58" s="47"/>
       <c r="B58" s="47"/>
       <c r="C58" s="48"/>
       <c r="D58" s="43"/>
       <c r="E58" s="44"/>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="37"/>
       <c r="D59" s="32"/>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="27"/>
       <c r="D60" s="28"/>
       <c r="E60" s="15"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="31"/>
       <c r="D61" s="32"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="33"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="47"/>
       <c r="B63" s="47"/>
       <c r="C63" s="63"/>
       <c r="D63" s="43"/>
       <c r="E63" s="58"/>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="31" t="s">
@@ -1825,7 +1839,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="59" t="s">
@@ -1838,7 +1852,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="31" t="s">
@@ -1851,7 +1865,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.25" customHeight="1">
+    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="27"/>
@@ -1860,18 +1874,18 @@
       <c r="G67" s="50"/>
       <c r="H67" s="50"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="33"/>
       <c r="B68" s="33"/>
-      <c r="C68" s="73" t="s">
+      <c r="C68" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="73"/>
+      <c r="D68" s="74"/>
       <c r="E68" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="16"/>
       <c r="B69" s="16"/>
       <c r="C69" s="37" t="s">
@@ -1884,21 +1898,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="C70" s="27"/>
       <c r="D70" s="28"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="16"/>
       <c r="B71" s="16"/>
       <c r="C71" s="37"/>
       <c r="D71" s="38"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.25" customHeight="1">
+    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="C72" s="27"/>
@@ -1907,19 +1921,19 @@
       <c r="G72" s="50"/>
       <c r="H72" s="50"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="33"/>
       <c r="B73" s="33"/>
-      <c r="C73" s="73" t="s">
+      <c r="C73" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="73"/>
+      <c r="D73" s="74"/>
       <c r="E73" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G73" s="51"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
       <c r="C74" s="31" t="s">
@@ -1933,7 +1947,7 @@
       </c>
       <c r="G74" s="51"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="27" t="s">
@@ -1947,7 +1961,7 @@
       </c>
       <c r="G75" s="51"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="29" t="s">
@@ -1961,7 +1975,7 @@
       </c>
       <c r="G76" s="51"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="27" t="s">
@@ -1975,13 +1989,13 @@
       </c>
       <c r="G77" s="51"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="33"/>
       <c r="B78" s="33"/>
-      <c r="C78" s="73" t="s">
+      <c r="C78" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="73"/>
+      <c r="D78" s="74"/>
       <c r="E78" s="9" t="s">
         <v>39</v>
       </c>
@@ -2064,7 +2078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
       <c r="C84" s="59" t="s">
@@ -2077,7 +2091,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.25" customHeight="1">
+    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.35" customHeight="1">
       <c r="A85" s="53"/>
       <c r="B85" s="53"/>
       <c r="C85" s="64"/>
@@ -2085,14 +2099,14 @@
       <c r="E85" s="66"/>
       <c r="F85" s="67"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="C86" s="59"/>
       <c r="D86" s="61"/>
       <c r="E86" s="58"/>
     </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="16"/>
       <c r="C87" s="31"/>
@@ -2100,7 +2114,7 @@
       <c r="E87" s="60"/>
       <c r="F87" s="51"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="59"/>
@@ -2115,14 +2129,14 @@
       <c r="E89" s="52"/>
       <c r="F89" s="51"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="C90" s="59"/>
       <c r="D90" s="61"/>
       <c r="E90" s="58"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="16"/>
       <c r="C91" s="31"/>
@@ -2130,14 +2144,14 @@
       <c r="E91" s="60"/>
       <c r="F91" s="51"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="C92" s="59"/>
       <c r="D92" s="61"/>
       <c r="E92" s="58"/>
     </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="16"/>
       <c r="C93" s="31"/>
@@ -2145,7 +2159,7 @@
       <c r="E93" s="60"/>
       <c r="F93" s="51"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="C94" s="59"/>
@@ -2167,7 +2181,7 @@
       <c r="D96" s="28"/>
       <c r="E96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="16"/>
       <c r="C97" s="29"/>
@@ -2175,26 +2189,26 @@
       <c r="E97" s="19"/>
       <c r="F97" s="51"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="C98" s="27"/>
       <c r="D98" s="28"/>
       <c r="E98" s="15"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="33"/>
       <c r="B99" s="33"/>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D99" s="73"/>
+      <c r="D99" s="74"/>
       <c r="E99" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G99" s="51"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="16"/>
       <c r="B100" s="16"/>
       <c r="C100" s="52" t="s">
@@ -2207,14 +2221,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="C101" s="27"/>
       <c r="D101" s="28"/>
       <c r="E101" s="15"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="33"/>
       <c r="B102" s="33"/>
       <c r="C102" s="34" t="s">
@@ -2225,7 +2239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="31" t="s">
@@ -2238,7 +2252,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="C104" s="59" t="s">
@@ -2251,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="37" t="s">
@@ -2264,7 +2278,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="C106" s="27" t="s">
@@ -2277,21 +2291,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="31"/>
       <c r="D107" s="32"/>
       <c r="E107" s="60"/>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="C108" s="27"/>
       <c r="D108" s="28"/>
       <c r="E108" s="15"/>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="29" t="s">
@@ -2304,7 +2318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="C110" s="27" t="s">
@@ -2317,7 +2331,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="29" t="s">
@@ -2330,7 +2344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="C112" s="27" t="s">
@@ -2343,14 +2357,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="69"/>
       <c r="D113" s="65"/>
       <c r="E113" s="66"/>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
       <c r="C114" s="59" t="s">
@@ -2363,7 +2377,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="16"/>
       <c r="B115" s="16"/>
       <c r="C115" s="31" t="s">
@@ -2376,7 +2390,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="25.5">
       <c r="A116" s="20"/>
       <c r="B116" s="20"/>
       <c r="C116" s="59" t="s">
@@ -2389,14 +2403,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="16"/>
       <c r="B117" s="16"/>
       <c r="C117" s="31"/>
       <c r="D117" s="32"/>
       <c r="E117" s="60"/>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="20"/>
       <c r="B118" s="20"/>
       <c r="C118" s="59" t="s">
@@ -2435,63 +2449,63 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="16"/>
       <c r="B121" s="16"/>
       <c r="C121" s="37"/>
       <c r="D121" s="38"/>
       <c r="E121" s="19"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="20"/>
       <c r="B122" s="20"/>
       <c r="C122" s="27"/>
       <c r="D122" s="28"/>
       <c r="E122" s="15"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="16"/>
       <c r="B123" s="16"/>
       <c r="C123" s="37"/>
       <c r="D123" s="38"/>
       <c r="E123" s="19"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="20"/>
       <c r="B124" s="20"/>
       <c r="C124" s="27"/>
       <c r="D124" s="28"/>
       <c r="E124" s="15"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="16"/>
       <c r="B125" s="16"/>
       <c r="C125" s="37"/>
       <c r="D125" s="38"/>
       <c r="E125" s="19"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="20"/>
       <c r="B126" s="20"/>
       <c r="C126" s="27"/>
       <c r="D126" s="28"/>
       <c r="E126" s="15"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="16"/>
       <c r="B127" s="16"/>
       <c r="C127" s="37"/>
       <c r="D127" s="38"/>
       <c r="E127" s="19"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="27"/>
       <c r="D128" s="28"/>
       <c r="E128" s="15"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="29" t="s">
@@ -2504,7 +2518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="27" t="s">
@@ -3394,11 +3408,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3406,6 +3415,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added red light sensor to hardware
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2023.xlsx
+++ b/Kilroy Equipment List 2023.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="150">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>0,1</t>
+  </si>
+  <si>
+    <t>redLightSensor</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>red light sensor - QS18VN6LV</t>
   </si>
 </sst>
 </file>
@@ -860,11 +869,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1175,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1186,33 +1195,32 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14:E14"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.6328125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="1"/>
-    <col min="8" max="8" width="11.08984375" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.90625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1229,13 +1237,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="21" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="21" customFormat="1">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="13" t="s">
@@ -1292,7 +1300,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
@@ -1302,7 +1310,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="59" t="s">
@@ -1318,7 +1326,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="31" t="s">
@@ -1334,7 +1342,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="59" t="s">
@@ -1347,7 +1355,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="31" t="s">
@@ -1363,21 +1371,21 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="59"/>
       <c r="D13" s="61"/>
       <c r="E13" s="58"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="60"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="59" t="s">
@@ -1390,7 +1398,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="31" t="s">
@@ -1403,49 +1411,49 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="59"/>
       <c r="D17" s="61"/>
       <c r="E17" s="58"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="62"/>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="19" spans="1:8" s="4" customFormat="1">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="59"/>
       <c r="D19" s="61"/>
       <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="46"/>
       <c r="D20" s="70"/>
       <c r="E20" s="62"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="59"/>
       <c r="D21" s="61"/>
       <c r="E21" s="58"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="46"/>
       <c r="D22" s="70"/>
       <c r="E22" s="62"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="33"/>
       <c r="C23" s="75" t="s">
@@ -1456,21 +1464,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="58"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="C24" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="31"/>
       <c r="D25" s="32"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="59"/>
@@ -1480,7 +1494,7 @@
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="31"/>
@@ -1490,7 +1504,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="28" spans="1:8" s="4" customFormat="1">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="59"/>
@@ -1500,7 +1514,7 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="31"/>
@@ -1510,7 +1524,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="27"/>
@@ -1520,7 +1534,7 @@
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="37"/>
@@ -1530,18 +1544,18 @@
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="73"/>
+      <c r="D32" s="74"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="36"/>
       <c r="B33" s="36"/>
       <c r="C33" s="27" t="s">
@@ -1554,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="31" t="s">
@@ -1567,7 +1581,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="59" t="s">
@@ -1580,81 +1594,81 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="29"/>
       <c r="D36" s="30"/>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="31"/>
       <c r="D38" s="40"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="29"/>
       <c r="D40" s="30"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="37"/>
       <c r="D42" s="38"/>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="27"/>
       <c r="D43" s="28"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="29"/>
       <c r="D44" s="30"/>
       <c r="E44" s="19"/>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="73"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="42" t="s">
         <v>14</v>
       </c>
@@ -1672,7 +1686,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="29"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="20" t="s">
         <v>14</v>
       </c>
@@ -1683,25 +1697,25 @@
       <c r="D48" s="28"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="37"/>
       <c r="D49" s="38"/>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.15" customHeight="1">
+    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.1" customHeight="1">
       <c r="A51" s="47"/>
       <c r="B51" s="47"/>
       <c r="C51" s="63" t="s">
@@ -1714,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="53"/>
       <c r="B52" s="53"/>
       <c r="C52" s="69" t="s">
@@ -1727,92 +1741,92 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="27"/>
       <c r="D53" s="28"/>
       <c r="E53" s="15"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="16"/>
       <c r="B54" s="16"/>
       <c r="C54" s="31"/>
       <c r="D54" s="32"/>
       <c r="E54" s="11"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="27"/>
       <c r="D55" s="28"/>
       <c r="E55" s="15"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="31"/>
       <c r="D56" s="32"/>
       <c r="E56" s="11"/>
     </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A57" s="33"/>
       <c r="B57" s="33"/>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.25" customHeight="1">
+    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
       <c r="A58" s="47"/>
       <c r="B58" s="47"/>
       <c r="C58" s="48"/>
       <c r="D58" s="43"/>
       <c r="E58" s="44"/>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="37"/>
       <c r="D59" s="32"/>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="27"/>
       <c r="D60" s="28"/>
       <c r="E60" s="15"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="31"/>
       <c r="D61" s="32"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="33"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="47"/>
       <c r="B63" s="47"/>
       <c r="C63" s="63"/>
       <c r="D63" s="43"/>
       <c r="E63" s="58"/>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="31" t="s">
@@ -1825,7 +1839,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="59" t="s">
@@ -1838,7 +1852,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="31" t="s">
@@ -1851,7 +1865,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.25" customHeight="1">
+    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="27"/>
@@ -1860,18 +1874,18 @@
       <c r="G67" s="50"/>
       <c r="H67" s="50"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="33"/>
       <c r="B68" s="33"/>
-      <c r="C68" s="73" t="s">
+      <c r="C68" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="73"/>
+      <c r="D68" s="74"/>
       <c r="E68" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="16"/>
       <c r="B69" s="16"/>
       <c r="C69" s="37" t="s">
@@ -1884,21 +1898,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="C70" s="27"/>
       <c r="D70" s="28"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="16"/>
       <c r="B71" s="16"/>
       <c r="C71" s="37"/>
       <c r="D71" s="38"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.25" customHeight="1">
+    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="C72" s="27"/>
@@ -1907,19 +1921,19 @@
       <c r="G72" s="50"/>
       <c r="H72" s="50"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="33"/>
       <c r="B73" s="33"/>
-      <c r="C73" s="73" t="s">
+      <c r="C73" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="73"/>
+      <c r="D73" s="74"/>
       <c r="E73" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G73" s="51"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
       <c r="C74" s="31" t="s">
@@ -1933,7 +1947,7 @@
       </c>
       <c r="G74" s="51"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="27" t="s">
@@ -1947,7 +1961,7 @@
       </c>
       <c r="G75" s="51"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="29" t="s">
@@ -1961,7 +1975,7 @@
       </c>
       <c r="G76" s="51"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="27" t="s">
@@ -1975,13 +1989,13 @@
       </c>
       <c r="G77" s="51"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="33"/>
       <c r="B78" s="33"/>
-      <c r="C78" s="73" t="s">
+      <c r="C78" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="73"/>
+      <c r="D78" s="74"/>
       <c r="E78" s="9" t="s">
         <v>39</v>
       </c>
@@ -2064,7 +2078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
       <c r="C84" s="59" t="s">
@@ -2077,7 +2091,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.25" customHeight="1">
+    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.35" customHeight="1">
       <c r="A85" s="53"/>
       <c r="B85" s="53"/>
       <c r="C85" s="64"/>
@@ -2085,14 +2099,14 @@
       <c r="E85" s="66"/>
       <c r="F85" s="67"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="C86" s="59"/>
       <c r="D86" s="61"/>
       <c r="E86" s="58"/>
     </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="16"/>
       <c r="C87" s="31"/>
@@ -2100,7 +2114,7 @@
       <c r="E87" s="60"/>
       <c r="F87" s="51"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="59"/>
@@ -2115,14 +2129,14 @@
       <c r="E89" s="52"/>
       <c r="F89" s="51"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="C90" s="59"/>
       <c r="D90" s="61"/>
       <c r="E90" s="58"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="16"/>
       <c r="C91" s="31"/>
@@ -2130,14 +2144,14 @@
       <c r="E91" s="60"/>
       <c r="F91" s="51"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="C92" s="59"/>
       <c r="D92" s="61"/>
       <c r="E92" s="58"/>
     </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="16"/>
       <c r="C93" s="31"/>
@@ -2145,7 +2159,7 @@
       <c r="E93" s="60"/>
       <c r="F93" s="51"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="C94" s="59"/>
@@ -2167,7 +2181,7 @@
       <c r="D96" s="28"/>
       <c r="E96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.25" customHeight="1">
+    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="16"/>
       <c r="C97" s="29"/>
@@ -2175,26 +2189,26 @@
       <c r="E97" s="19"/>
       <c r="F97" s="51"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="C98" s="27"/>
       <c r="D98" s="28"/>
       <c r="E98" s="15"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="33"/>
       <c r="B99" s="33"/>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D99" s="73"/>
+      <c r="D99" s="74"/>
       <c r="E99" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G99" s="51"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="16"/>
       <c r="B100" s="16"/>
       <c r="C100" s="52" t="s">
@@ -2207,14 +2221,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="C101" s="27"/>
       <c r="D101" s="28"/>
       <c r="E101" s="15"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="33"/>
       <c r="B102" s="33"/>
       <c r="C102" s="34" t="s">
@@ -2225,7 +2239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="31" t="s">
@@ -2238,7 +2252,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="C104" s="59" t="s">
@@ -2251,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="37" t="s">
@@ -2264,7 +2278,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="C106" s="27" t="s">
@@ -2277,21 +2291,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="31"/>
       <c r="D107" s="32"/>
       <c r="E107" s="60"/>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="C108" s="27"/>
       <c r="D108" s="28"/>
       <c r="E108" s="15"/>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="29" t="s">
@@ -2304,7 +2318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="C110" s="27" t="s">
@@ -2317,7 +2331,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="29" t="s">
@@ -2330,7 +2344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="C112" s="27" t="s">
@@ -2343,14 +2357,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="69"/>
       <c r="D113" s="65"/>
       <c r="E113" s="66"/>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
       <c r="C114" s="59" t="s">
@@ -2363,7 +2377,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="16"/>
       <c r="B115" s="16"/>
       <c r="C115" s="31" t="s">
@@ -2376,7 +2390,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="25.5">
       <c r="A116" s="20"/>
       <c r="B116" s="20"/>
       <c r="C116" s="59" t="s">
@@ -2389,14 +2403,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="16"/>
       <c r="B117" s="16"/>
       <c r="C117" s="31"/>
       <c r="D117" s="32"/>
       <c r="E117" s="60"/>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="20"/>
       <c r="B118" s="20"/>
       <c r="C118" s="59" t="s">
@@ -2435,63 +2449,63 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="16"/>
       <c r="B121" s="16"/>
       <c r="C121" s="37"/>
       <c r="D121" s="38"/>
       <c r="E121" s="19"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="20"/>
       <c r="B122" s="20"/>
       <c r="C122" s="27"/>
       <c r="D122" s="28"/>
       <c r="E122" s="15"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="16"/>
       <c r="B123" s="16"/>
       <c r="C123" s="37"/>
       <c r="D123" s="38"/>
       <c r="E123" s="19"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="20"/>
       <c r="B124" s="20"/>
       <c r="C124" s="27"/>
       <c r="D124" s="28"/>
       <c r="E124" s="15"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="16"/>
       <c r="B125" s="16"/>
       <c r="C125" s="37"/>
       <c r="D125" s="38"/>
       <c r="E125" s="19"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="20"/>
       <c r="B126" s="20"/>
       <c r="C126" s="27"/>
       <c r="D126" s="28"/>
       <c r="E126" s="15"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="16"/>
       <c r="B127" s="16"/>
       <c r="C127" s="37"/>
       <c r="D127" s="38"/>
       <c r="E127" s="19"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="27"/>
       <c r="D128" s="28"/>
       <c r="E128" s="15"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="29" t="s">
@@ -2504,7 +2518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="27" t="s">
@@ -3394,11 +3408,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3406,6 +3415,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added hardware for main 339 robot
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2023.xlsx
+++ b/Kilroy Equipment List 2023.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -453,9 +453,6 @@
     <t>armRaiseMotor</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>armRaiseMotor - CAN Venom</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>Red light sensor - QS18VN6LV</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -869,11 +869,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1184,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1195,32 +1195,32 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1237,13 +1237,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="21" customFormat="1">
+    <row r="7" spans="1:8" s="21" customFormat="1" ht="13">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="13" t="s">
@@ -1300,7 +1300,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
@@ -1310,7 +1310,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="59" t="s">
@@ -1326,7 +1326,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="31" t="s">
@@ -1342,7 +1342,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="59" t="s">
@@ -1355,7 +1355,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="31" t="s">
@@ -1371,25 +1371,25 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="59"/>
       <c r="D13" s="61"/>
       <c r="E13" s="58"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="60"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="61" t="s">
         <v>45</v>
@@ -1398,62 +1398,62 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>142</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="59"/>
       <c r="D17" s="61"/>
       <c r="E17" s="58"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="62"/>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1">
+    <row r="19" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="59"/>
       <c r="D19" s="61"/>
       <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="46"/>
       <c r="D20" s="70"/>
       <c r="E20" s="62"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="59"/>
       <c r="D21" s="61"/>
       <c r="E21" s="58"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="46"/>
       <c r="D22" s="70"/>
       <c r="E22" s="62"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="33"/>
       <c r="C23" s="75" t="s">
@@ -1464,27 +1464,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="58" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="31"/>
       <c r="D25" s="32"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="59"/>
@@ -1494,7 +1494,7 @@
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="31"/>
@@ -1504,7 +1504,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="59"/>
@@ -1514,7 +1514,7 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="31"/>
@@ -1524,7 +1524,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="27"/>
@@ -1534,7 +1534,7 @@
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="37"/>
@@ -1544,18 +1544,18 @@
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
-      <c r="C32" s="74" t="s">
+      <c r="C32" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="74"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A33" s="36"/>
       <c r="B33" s="36"/>
       <c r="C33" s="27" t="s">
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="31" t="s">
@@ -1581,7 +1581,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="59" t="s">
@@ -1594,81 +1594,81 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="29"/>
       <c r="D36" s="30"/>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="31"/>
       <c r="D38" s="40"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="29"/>
       <c r="D40" s="30"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
+    <row r="41" spans="1:5" s="41" customFormat="1" ht="13.4" customHeight="1">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="37"/>
       <c r="D42" s="38"/>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
+    <row r="43" spans="1:5" s="41" customFormat="1" ht="13.4" customHeight="1">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="27"/>
       <c r="D43" s="28"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
+    <row r="44" spans="1:5" s="41" customFormat="1" ht="13.4" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="29"/>
       <c r="D44" s="30"/>
       <c r="E44" s="19"/>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
-      <c r="C45" s="74" t="s">
+      <c r="C45" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="74"/>
+      <c r="D45" s="73"/>
       <c r="E45" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A46" s="42" t="s">
         <v>14</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="29"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A48" s="20" t="s">
         <v>14</v>
       </c>
@@ -1697,25 +1697,25 @@
       <c r="D48" s="28"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="37"/>
       <c r="D49" s="38"/>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="74"/>
+      <c r="D50" s="73"/>
       <c r="E50" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.1" customHeight="1">
+    <row r="51" spans="1:5" s="41" customFormat="1" ht="14.15" customHeight="1">
       <c r="A51" s="47"/>
       <c r="B51" s="47"/>
       <c r="C51" s="63" t="s">
@@ -1728,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A52" s="53"/>
       <c r="B52" s="53"/>
       <c r="C52" s="69" t="s">
@@ -1741,92 +1741,92 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="27"/>
       <c r="D53" s="28"/>
       <c r="E53" s="15"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A54" s="16"/>
       <c r="B54" s="16"/>
       <c r="C54" s="31"/>
       <c r="D54" s="32"/>
       <c r="E54" s="11"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="27"/>
       <c r="D55" s="28"/>
       <c r="E55" s="15"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="31"/>
       <c r="D56" s="32"/>
       <c r="E56" s="11"/>
     </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A57" s="33"/>
       <c r="B57" s="33"/>
-      <c r="C57" s="74" t="s">
+      <c r="C57" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="74"/>
+      <c r="D57" s="73"/>
       <c r="E57" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.35" customHeight="1">
+    <row r="58" spans="1:5" s="41" customFormat="1" ht="13.4" customHeight="1">
       <c r="A58" s="47"/>
       <c r="B58" s="47"/>
       <c r="C58" s="48"/>
       <c r="D58" s="43"/>
       <c r="E58" s="44"/>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="37"/>
       <c r="D59" s="32"/>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="27"/>
       <c r="D60" s="28"/>
       <c r="E60" s="15"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="31"/>
       <c r="D61" s="32"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="33"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="74" t="s">
+      <c r="C62" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="74"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A63" s="47"/>
       <c r="B63" s="47"/>
       <c r="C63" s="63"/>
       <c r="D63" s="43"/>
       <c r="E63" s="58"/>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="31" t="s">
@@ -1839,7 +1839,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="59" t="s">
@@ -1852,7 +1852,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="31" t="s">
@@ -1862,10 +1862,10 @@
         <v>127</v>
       </c>
       <c r="E66" s="60" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="49" customFormat="1" ht="13.4" customHeight="1">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="27"/>
@@ -1874,18 +1874,18 @@
       <c r="G67" s="50"/>
       <c r="H67" s="50"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="33"/>
       <c r="B68" s="33"/>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="74"/>
+      <c r="D68" s="73"/>
       <c r="E68" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A69" s="16"/>
       <c r="B69" s="16"/>
       <c r="C69" s="37" t="s">
@@ -1898,21 +1898,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="C70" s="27"/>
       <c r="D70" s="28"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A71" s="16"/>
       <c r="B71" s="16"/>
       <c r="C71" s="37"/>
       <c r="D71" s="38"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.35" customHeight="1">
+    <row r="72" spans="1:8" s="49" customFormat="1" ht="13.4" customHeight="1">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="C72" s="27"/>
@@ -1921,19 +1921,19 @@
       <c r="G72" s="50"/>
       <c r="H72" s="50"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="33"/>
       <c r="B73" s="33"/>
-      <c r="C73" s="74" t="s">
+      <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="74"/>
+      <c r="D73" s="73"/>
       <c r="E73" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G73" s="51"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
       <c r="C74" s="31" t="s">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="G74" s="51"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="27" t="s">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="G75" s="51"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="29" t="s">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="G76" s="51"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="27" t="s">
@@ -1989,13 +1989,13 @@
       </c>
       <c r="G77" s="51"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="33"/>
       <c r="B78" s="33"/>
-      <c r="C78" s="74" t="s">
+      <c r="C78" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="74"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="9" t="s">
         <v>39</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
       <c r="C84" s="59" t="s">
@@ -2091,7 +2091,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.35" customHeight="1">
+    <row r="85" spans="1:6" s="68" customFormat="1" ht="13.4" customHeight="1">
       <c r="A85" s="53"/>
       <c r="B85" s="53"/>
       <c r="C85" s="64"/>
@@ -2099,14 +2099,14 @@
       <c r="E85" s="66"/>
       <c r="F85" s="67"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="C86" s="59"/>
       <c r="D86" s="61"/>
       <c r="E86" s="58"/>
     </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="16"/>
       <c r="C87" s="31"/>
@@ -2114,7 +2114,7 @@
       <c r="E87" s="60"/>
       <c r="F87" s="51"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="59"/>
@@ -2129,14 +2129,14 @@
       <c r="E89" s="52"/>
       <c r="F89" s="51"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="C90" s="59"/>
       <c r="D90" s="61"/>
       <c r="E90" s="58"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="16"/>
       <c r="C91" s="31"/>
@@ -2144,14 +2144,14 @@
       <c r="E91" s="60"/>
       <c r="F91" s="51"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="C92" s="59"/>
       <c r="D92" s="61"/>
       <c r="E92" s="58"/>
     </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="16"/>
       <c r="C93" s="31"/>
@@ -2159,7 +2159,7 @@
       <c r="E93" s="60"/>
       <c r="F93" s="51"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="C94" s="59"/>
@@ -2181,7 +2181,7 @@
       <c r="D96" s="28"/>
       <c r="E96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="97" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="16"/>
       <c r="C97" s="29"/>
@@ -2189,26 +2189,26 @@
       <c r="E97" s="19"/>
       <c r="F97" s="51"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="C98" s="27"/>
       <c r="D98" s="28"/>
       <c r="E98" s="15"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="33"/>
       <c r="B99" s="33"/>
-      <c r="C99" s="74" t="s">
+      <c r="C99" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D99" s="74"/>
+      <c r="D99" s="73"/>
       <c r="E99" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G99" s="51"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A100" s="16"/>
       <c r="B100" s="16"/>
       <c r="C100" s="52" t="s">
@@ -2221,14 +2221,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="C101" s="27"/>
       <c r="D101" s="28"/>
       <c r="E101" s="15"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A102" s="33"/>
       <c r="B102" s="33"/>
       <c r="C102" s="34" t="s">
@@ -2239,7 +2239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="31" t="s">
@@ -2252,7 +2252,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="C104" s="59" t="s">
@@ -2265,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="37" t="s">
@@ -2278,7 +2278,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="C106" s="27" t="s">
@@ -2291,21 +2291,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="31"/>
       <c r="D107" s="32"/>
       <c r="E107" s="60"/>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="C108" s="27"/>
       <c r="D108" s="28"/>
       <c r="E108" s="15"/>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="29" t="s">
@@ -2318,7 +2318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="C110" s="27" t="s">
@@ -2331,7 +2331,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="29" t="s">
@@ -2344,7 +2344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="C112" s="27" t="s">
@@ -2357,14 +2357,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="69"/>
       <c r="D113" s="65"/>
       <c r="E113" s="66"/>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
       <c r="C114" s="59" t="s">
@@ -2377,7 +2377,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A115" s="16"/>
       <c r="B115" s="16"/>
       <c r="C115" s="31" t="s">
@@ -2390,7 +2390,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="25.5">
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="20"/>
       <c r="B116" s="20"/>
       <c r="C116" s="59" t="s">
@@ -2403,14 +2403,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
+    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A117" s="16"/>
       <c r="B117" s="16"/>
       <c r="C117" s="31"/>
       <c r="D117" s="32"/>
       <c r="E117" s="60"/>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
+    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A118" s="20"/>
       <c r="B118" s="20"/>
       <c r="C118" s="59" t="s">
@@ -2449,63 +2449,63 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
+    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A121" s="16"/>
       <c r="B121" s="16"/>
       <c r="C121" s="37"/>
       <c r="D121" s="38"/>
       <c r="E121" s="19"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
+    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A122" s="20"/>
       <c r="B122" s="20"/>
       <c r="C122" s="27"/>
       <c r="D122" s="28"/>
       <c r="E122" s="15"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A123" s="16"/>
       <c r="B123" s="16"/>
       <c r="C123" s="37"/>
       <c r="D123" s="38"/>
       <c r="E123" s="19"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1">
+    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A124" s="20"/>
       <c r="B124" s="20"/>
       <c r="C124" s="27"/>
       <c r="D124" s="28"/>
       <c r="E124" s="15"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1">
+    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A125" s="16"/>
       <c r="B125" s="16"/>
       <c r="C125" s="37"/>
       <c r="D125" s="38"/>
       <c r="E125" s="19"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
+    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A126" s="20"/>
       <c r="B126" s="20"/>
       <c r="C126" s="27"/>
       <c r="D126" s="28"/>
       <c r="E126" s="15"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
+    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A127" s="16"/>
       <c r="B127" s="16"/>
       <c r="C127" s="37"/>
       <c r="D127" s="38"/>
       <c r="E127" s="19"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
+    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="27"/>
       <c r="D128" s="28"/>
       <c r="E128" s="15"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="29" t="s">
@@ -2518,7 +2518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
+    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="27" t="s">
@@ -3408,6 +3408,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3415,11 +3420,6 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>